<commit_message>
bugfix: unit converstions. Cuz always
</commit_message>
<xml_diff>
--- a/LPR_pycap_opt/Student_Input/LPR_Single_Run.xlsx
+++ b/LPR_pycap_opt/Student_Input/LPR_Single_Run.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mnfienen/Documents/GIT/LPR_redux/LPR_pycap_opt/Student_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5873902D-5C89-564E-8F24-E76D972779F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B45E80-4D41-5240-A8A1-09B689C48DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="7300" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{281DC555-9697-4BFF-9DD7-77B5DC79D066}"/>
   </bookViews>
@@ -856,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3486D8CF-98E7-4C21-B0E2-2FCF4CCA21CC}">
   <dimension ref="A1:H328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H151" sqref="H151"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1256,7 +1256,7 @@
         <v>42</v>
       </c>
       <c r="G15" s="4">
-        <v>76.2</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <v>30</v>
@@ -1282,7 +1282,7 @@
         <v>36</v>
       </c>
       <c r="G16" s="4">
-        <v>222.8</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <v>90</v>
@@ -2719,7 +2719,7 @@
         <v>42</v>
       </c>
       <c r="G73" s="4">
-        <v>275.8</v>
+        <v>0</v>
       </c>
       <c r="H73">
         <v>120</v>
@@ -3143,7 +3143,7 @@
         <v>42</v>
       </c>
       <c r="G90" s="4">
-        <v>1133.7</v>
+        <v>0</v>
       </c>
       <c r="H90">
         <v>90</v>
@@ -3498,7 +3498,7 @@
         <v>42</v>
       </c>
       <c r="G104" s="4">
-        <v>216.9</v>
+        <v>0</v>
       </c>
       <c r="H104">
         <v>120</v>

</xml_diff>